<commit_message>
Fixed errors of dataprovider
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_TestData.xlsx
+++ b/testdata/Scenario1_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408439\CTS_Java_Training\Practicals\IntelliJ_Selenium_Projects\Hackathon_Project\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC2FBB6-6857-48FA-9533-7F13BF3A0E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FECD31-5D49-47B1-82A3-40CB1AFB5439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>TC_ID</t>
   </si>
@@ -95,9 +95,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>2 Travellers(s)</t>
-  </si>
-  <si>
     <t>validateClickingOnViewPlansAndGoingToPlansPage</t>
   </si>
   <si>
@@ -156,6 +153,42 @@
   </si>
   <si>
     <t>TC_010</t>
+  </si>
+  <si>
+    <t>Automation Test Script ID</t>
+  </si>
+  <si>
+    <t>ATC001</t>
+  </si>
+  <si>
+    <t>ATC002</t>
+  </si>
+  <si>
+    <t>ATC003</t>
+  </si>
+  <si>
+    <t>ATC004</t>
+  </si>
+  <si>
+    <t>ATC005</t>
+  </si>
+  <si>
+    <t>ATC006</t>
+  </si>
+  <si>
+    <t>ATC007</t>
+  </si>
+  <si>
+    <t>ATC008</t>
+  </si>
+  <si>
+    <t>ATC009</t>
+  </si>
+  <si>
+    <t>ATC010</t>
+  </si>
+  <si>
+    <t>2 Traveller(s)</t>
   </si>
 </sst>
 </file>
@@ -546,275 +579,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3050-D1DC-49F4-900E-5DA4D3857D18}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
-    <col min="7" max="7" width="19.6328125" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="42.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="H11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>